<commit_message>
cleaned datasets + excel files + re
</commit_message>
<xml_diff>
--- a/cleaned_dataset/coffee_trade.xlsx
+++ b/cleaned_dataset/coffee_trade.xlsx
@@ -395,88 +395,88 @@
     <t>European Union</t>
   </si>
   <si>
-    <t xml:space="preserve">   Austria</t>
+    <t>Austria</t>
   </si>
   <si>
-    <t xml:space="preserve">   Belgium</t>
+    <t>Belgium</t>
   </si>
   <si>
-    <t xml:space="preserve">   Belgium/Luxembourg</t>
+    <t>Belgium/Luxembourg</t>
   </si>
   <si>
-    <t xml:space="preserve">   Bulgaria</t>
+    <t>Bulgaria</t>
   </si>
   <si>
-    <t xml:space="preserve">   Croatia</t>
+    <t>Croatia</t>
   </si>
   <si>
-    <t xml:space="preserve">   Cyprus</t>
+    <t>Cyprus</t>
   </si>
   <si>
-    <t xml:space="preserve">   Czechia</t>
+    <t>Czechia</t>
   </si>
   <si>
-    <t xml:space="preserve">   Denmark</t>
+    <t>Denmark</t>
   </si>
   <si>
-    <t xml:space="preserve">   Estonia</t>
+    <t>Estonia</t>
   </si>
   <si>
-    <t xml:space="preserve">   Finland</t>
+    <t>Finland</t>
   </si>
   <si>
-    <t xml:space="preserve">   France</t>
+    <t>France</t>
   </si>
   <si>
-    <t xml:space="preserve">   Germany</t>
+    <t>Germany</t>
   </si>
   <si>
-    <t xml:space="preserve">   Greece</t>
+    <t>Greece</t>
   </si>
   <si>
-    <t xml:space="preserve">   Hungary</t>
+    <t>Hungary</t>
   </si>
   <si>
-    <t xml:space="preserve">   Ireland</t>
+    <t>Ireland</t>
   </si>
   <si>
-    <t xml:space="preserve">   Italy</t>
+    <t>Italy</t>
   </si>
   <si>
-    <t xml:space="preserve">   Latvia</t>
+    <t>Latvia</t>
   </si>
   <si>
-    <t xml:space="preserve">   Lithuania</t>
+    <t>Lithuania</t>
   </si>
   <si>
-    <t xml:space="preserve">   Luxembourg</t>
+    <t>Luxembourg</t>
   </si>
   <si>
-    <t xml:space="preserve">   Malta</t>
+    <t>Malta</t>
   </si>
   <si>
-    <t xml:space="preserve">   Netherlands</t>
+    <t>Netherlands</t>
   </si>
   <si>
-    <t xml:space="preserve">   Poland</t>
+    <t>Poland</t>
   </si>
   <si>
-    <t xml:space="preserve">   Portugal</t>
+    <t>Portugal</t>
   </si>
   <si>
-    <t xml:space="preserve">   Romania</t>
+    <t>Romania</t>
   </si>
   <si>
-    <t xml:space="preserve">   Slovakia</t>
+    <t>Slovakia</t>
   </si>
   <si>
-    <t xml:space="preserve">   Slovenia</t>
+    <t>Slovenia</t>
   </si>
   <si>
-    <t xml:space="preserve">   Spain</t>
+    <t>Spain</t>
   </si>
   <si>
-    <t xml:space="preserve">   Sweden</t>
+    <t>Sweden</t>
   </si>
   <si>
     <t>Japan</t>

</xml_diff>